<commit_message>
update peer review score
</commit_message>
<xml_diff>
--- a/P3/P3_PeerReview.xlsx
+++ b/P3/P3_PeerReview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TTU-CS\Github\CS5331_Spring2019\P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2467EA-D24E-41DE-BC7B-C06A86A36B0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAE214E-7DD3-4808-9EE4-7A57BEE5A0AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{5E94E157-D904-4DD4-8FF9-3E443BED4110}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Group</t>
   </si>
@@ -145,14 +145,6 @@
   </si>
   <si>
     <t>Team Member: David Cooper.   Rate: 5/5  David was a good choice to work with for both projects. His work on the preprocessing was crucial. His knowledge of these topics is huge and he is always super positive and helpful.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandon Stehling: 
-1
-didn't do much but was there to try and help when asked.
-Matthew Hendrick
-2
-did the map but that's it. seemed on top of things but didn't actually do much. </t>
   </si>
   <si>
     <t xml:space="preserve">Indiana Cooper (4): He contributed greatly to the report, and the front end code for our UI. </t>
@@ -315,6 +307,24 @@
 Arturo Mora: 5
 Mia Lyn Ward: 5
 Both Arturo and Mia worked on the parts they were assign and turn in progress on time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandon Stehling: 
+2
+didn't do much but was there to try and help when asked.
+Matthew Hendrick
+3
+did the map but that's it. seemed on top of things but didn't actually do much. </t>
+  </si>
+  <si>
+    <t>Lino Virgen
+Rating: 5/5
+Review:
+Lino was our team leader and did his fair share of the work. He was great to work with, and he held me accountable to my share of the work.
+Alexander Tesfazgi
+Rating: 4.5/5
+Review:
+Alexander did his fair share of the work, but I didn't see him much during our scheduled class time. I do know he was in communication with Lino outside of class, but it would have been nice to discuss the project more with all three of us there.</t>
   </si>
 </sst>
 </file>
@@ -681,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E895BF0F-A436-4AA9-BB43-4FAEB3E2D715}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -718,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -740,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +770,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,7 +799,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -811,7 +821,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,7 +832,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="180" x14ac:dyDescent="0.25">
@@ -833,7 +843,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -844,7 +854,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="360" x14ac:dyDescent="0.25">
@@ -855,7 +865,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -866,7 +876,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
@@ -877,7 +887,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -888,7 +898,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -899,7 +909,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -910,7 +920,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -921,7 +931,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -932,7 +942,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -943,7 +953,7 @@
         <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -954,15 +964,18 @@
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -973,7 +986,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,7 +1005,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1012,7 +1025,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="180" x14ac:dyDescent="0.25">
@@ -1023,7 +1036,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1034,7 +1047,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,7 +1074,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>